<commit_message>
Corrected some mistakes in the analysis for both 1948 & 2022. The values in the excel table for 1948 were also incorrect, they have been corrected.
</commit_message>
<xml_diff>
--- a/Fide1948.xlsx
+++ b/Fide1948.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autuni-my.sharepoint.com/personal/cdk6032_autuni_ac_nz/Documents/Documents/Academic Life/Master of Analytics/ENGE817 STEM Research paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{D6EF6B64-29D6-46B9-A33D-2A2C59B1C1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CEA0080-9464-4146-BEC9-BBF41A998247}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{D6EF6B64-29D6-46B9-A33D-2A2C59B1C1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFE4BD1D-1250-4DF1-9D53-1CD076B40DCB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0155357F-FFFF-477A-A0D1-3639DE08C7F0}"/>
+    <workbookView xWindow="5892" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{0155357F-FFFF-477A-A0D1-3639DE08C7F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="11">
   <si>
     <t>Round</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Botvinnik</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vs Smy</t>
   </si>
 </sst>
 </file>
@@ -195,7 +192,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AEC80834-514B-40DE-99D1-AB2A7047DAB4}" name="Table1" displayName="Table1" ref="A1:F52" totalsRowCount="1" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:F51" xr:uid="{AEC80834-514B-40DE-99D1-AB2A7047DAB4}"/>
+  <autoFilter ref="A1:F51" xr:uid="{AEC80834-514B-40DE-99D1-AB2A7047DAB4}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Euwe"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6B165BC2-F437-4ED4-B75A-B1EC2A7A9826}" name="Round"/>
     <tableColumn id="2" xr3:uid="{A5629B3A-91A0-46DD-AA48-92315D760276}" name="WhitePlayer"/>
@@ -508,7 +511,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +557,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -571,7 +574,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -588,7 +591,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -605,7 +608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -622,7 +625,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -639,7 +642,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -673,7 +676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -690,7 +693,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -707,7 +710,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -724,7 +727,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -758,7 +761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -775,7 +778,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -792,7 +795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -809,7 +812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -826,7 +829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -860,7 +863,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -877,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -911,7 +914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -928,7 +931,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -945,7 +948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -962,12 +965,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -976,165 +979,165 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F28">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
+    <row r="33" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
         <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32">
-        <v>0.5</v>
-      </c>
-      <c r="E32">
-        <v>0.5</v>
-      </c>
-      <c r="F32">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>42</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
@@ -1146,49 +1149,49 @@
         <v>0.5</v>
       </c>
       <c r="F37">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1197,29 +1200,29 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1231,49 +1234,49 @@
         <v>0.5</v>
       </c>
       <c r="F42">
-        <v>24</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F44">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D45">
         <v>0.5</v>
@@ -1282,41 +1285,41 @@
         <v>0.5</v>
       </c>
       <c r="F45">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F46">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F47">
-        <v>52</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
@@ -1324,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1333,15 +1336,15 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1350,41 +1353,41 @@
         <v>0</v>
       </c>
       <c r="F49">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50">
-        <v>0.5</v>
-      </c>
-      <c r="E50">
-        <v>0.5</v>
-      </c>
-      <c r="F50">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>